<commit_message>
tweaking figures and tables
</commit_message>
<xml_diff>
--- a/Brock-et-al_Tables.xlsx
+++ b/Brock-et-al_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/BCM/Projects/Bike-Injuries/Manuscript/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="717" documentId="8_{BE5EE19E-B02E-485F-AE94-93E3DB24DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C146251-03F4-4972-8AB0-D7B0EA4361D2}"/>
+  <xr:revisionPtr revIDLastSave="732" documentId="8_{BE5EE19E-B02E-485F-AE94-93E3DB24DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{220AA3D4-8AB4-4083-A918-277EB97F873B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{45F7941F-18C6-45A1-BF41-0E39AC7E3252}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{45F7941F-18C6-45A1-BF41-0E39AC7E3252}"/>
   </bookViews>
   <sheets>
     <sheet name="table1_demographics" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="293">
   <si>
     <t>Male</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Intoxicated</t>
   </si>
   <si>
-    <t>p</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -518,9 +515,6 @@
     <t>9 (0.2)</t>
   </si>
   <si>
-    <t>Hosipital-acquired Pneumonia</t>
-  </si>
-  <si>
     <t>159 (0.5)</t>
   </si>
   <si>
@@ -569,9 +563,6 @@
     <t>1556 (27.3)</t>
   </si>
   <si>
-    <t>Smoker</t>
-  </si>
-  <si>
     <t>3829 (11.0)</t>
   </si>
   <si>
@@ -678,9 +669,6 @@
   </si>
   <si>
     <t>100 (1.8)</t>
-  </si>
-  <si>
-    <t>Cirrosis</t>
   </si>
   <si>
     <t>119 (0.3)</t>
@@ -933,6 +921,15 @@
   </si>
   <si>
     <t>1.32 (1.20-1.46, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>Cirrhosis</t>
+  </si>
+  <si>
+    <t>Hospital-acquired Pneumonia</t>
+  </si>
+  <si>
+    <t>p-value</t>
   </si>
 </sst>
 </file>
@@ -983,15 +980,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1308,20 +1306,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE2C4BC-BC7A-4F93-BCA5-5502F54D71CA}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="C1" s="3" t="s">
         <v>24</v>
@@ -1333,170 +1332,170 @@
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
       <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>49</v>
       </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>58</v>
       </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1504,94 +1503,94 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>61</v>
       </c>
-      <c r="E12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>64</v>
       </c>
-      <c r="E13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>67</v>
       </c>
-      <c r="E14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>70</v>
       </c>
-      <c r="E15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
         <v>72</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>73</v>
       </c>
-      <c r="E16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" t="s">
         <v>75</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="E17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1599,31 +1598,31 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
         <v>78</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>79</v>
       </c>
-      <c r="E18" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>82</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>83</v>
-      </c>
-      <c r="E19" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1633,22 +1632,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71AEDE1F-E4AE-413B-AEE4-8AA0C81FA016}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
@@ -1659,693 +1659,669 @@
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>91</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>94</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>95</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>96</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="4">
+        <v>0.17100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F4">
-        <v>0.17100000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" t="s">
         <v>98</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="4">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E5" t="s">
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
         <v>100</v>
       </c>
-      <c r="F5">
-        <v>6.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" t="s">
         <v>102</v>
       </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>103</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>105</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>106</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>107</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>109</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>111</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>112</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>113</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>115</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>116</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>117</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>119</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>120</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>121</v>
       </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" t="s">
         <v>123</v>
       </c>
-      <c r="D12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
         <v>125</v>
       </c>
-      <c r="B13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>126</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>127</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" t="s">
         <v>129</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>130</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>131</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>132</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C20" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F21" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" t="s">
+        <v>197</v>
+      </c>
+      <c r="E22" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D23" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" t="s">
+        <v>202</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" t="s">
+        <v>205</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>209</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>290</v>
+      </c>
+      <c r="C26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" t="s">
+        <v>211</v>
+      </c>
+      <c r="E26" t="s">
+        <v>212</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D27" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" t="s">
+        <v>216</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" t="s">
         <v>133</v>
       </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" t="s">
-        <v>175</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" t="s">
-        <v>178</v>
-      </c>
-      <c r="E16" t="s">
-        <v>179</v>
-      </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C17" t="s">
-        <v>181</v>
-      </c>
-      <c r="D17" t="s">
-        <v>182</v>
-      </c>
-      <c r="E17" t="s">
-        <v>183</v>
-      </c>
-      <c r="F17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C19" t="s">
-        <v>189</v>
-      </c>
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" t="s">
-        <v>190</v>
-      </c>
-      <c r="F19">
-        <v>0.51400000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
-        <v>193</v>
-      </c>
-      <c r="F20">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C21" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" t="s">
-        <v>196</v>
-      </c>
-      <c r="E21" t="s">
-        <v>197</v>
-      </c>
-      <c r="F21">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" t="s">
-        <v>200</v>
-      </c>
-      <c r="E22" t="s">
-        <v>201</v>
-      </c>
-      <c r="F22">
-        <v>0.46200000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" t="s">
-        <v>203</v>
-      </c>
-      <c r="D23" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23" t="s">
-        <v>205</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C24" t="s">
-        <v>207</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.70799999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" t="s">
+        <v>151</v>
+      </c>
+      <c r="D33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>154</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="4">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" t="s">
         <v>161</v>
       </c>
-      <c r="E24" t="s">
-        <v>208</v>
-      </c>
-      <c r="F24">
-        <v>0.33100000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C25" t="s">
-        <v>210</v>
-      </c>
-      <c r="D25" t="s">
-        <v>211</v>
-      </c>
-      <c r="E25" t="s">
-        <v>212</v>
-      </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C26" t="s">
-        <v>214</v>
-      </c>
-      <c r="D26" t="s">
-        <v>215</v>
-      </c>
-      <c r="E26" t="s">
-        <v>216</v>
-      </c>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C27" t="s">
-        <v>218</v>
-      </c>
-      <c r="D27" t="s">
-        <v>219</v>
-      </c>
-      <c r="E27" t="s">
-        <v>220</v>
-      </c>
-      <c r="F27">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B28" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D37" t="s">
         <v>135</v>
       </c>
-      <c r="D28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E28" t="s">
-        <v>137</v>
-      </c>
-      <c r="F28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" t="s">
-        <v>140</v>
-      </c>
-      <c r="F29">
-        <v>5.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" t="s">
-        <v>143</v>
-      </c>
-      <c r="F30">
-        <v>0.70799999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>144</v>
-      </c>
-      <c r="C31" t="s">
-        <v>145</v>
-      </c>
-      <c r="D31" t="s">
-        <v>146</v>
-      </c>
-      <c r="E31" t="s">
-        <v>147</v>
-      </c>
-      <c r="F31">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>151</v>
-      </c>
-      <c r="C33" t="s">
-        <v>152</v>
-      </c>
-      <c r="D33" t="s">
-        <v>146</v>
-      </c>
-      <c r="E33" t="s">
-        <v>153</v>
-      </c>
-      <c r="F33">
-        <v>0.99399999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="E37" t="s">
+        <v>162</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" t="s">
         <v>135</v>
       </c>
-      <c r="D34" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" t="s">
-        <v>155</v>
-      </c>
-      <c r="F34">
-        <v>0.38500000000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>156</v>
-      </c>
-      <c r="C35" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" t="s">
-        <v>158</v>
-      </c>
-      <c r="F35">
-        <v>0.84199999999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>159</v>
-      </c>
-      <c r="C36" t="s">
-        <v>160</v>
-      </c>
-      <c r="D36" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36">
-        <v>0.189</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>162</v>
-      </c>
-      <c r="C37" t="s">
-        <v>163</v>
-      </c>
-      <c r="D37" t="s">
-        <v>136</v>
-      </c>
-      <c r="E37" t="s">
-        <v>164</v>
-      </c>
-      <c r="F37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="E38" t="s">
         <v>165</v>
       </c>
-      <c r="C38" t="s">
+      <c r="F38" s="4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>166</v>
       </c>
-      <c r="D38" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="C39" t="s">
         <v>167</v>
       </c>
-      <c r="F38">
-        <v>8.7999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>168</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>169</v>
       </c>
-      <c r="D39" t="s">
-        <v>170</v>
-      </c>
-      <c r="E39" t="s">
-        <v>171</v>
-      </c>
-      <c r="F39">
+      <c r="F39" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="4"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="4"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="4"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="4"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="4"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2357,19 +2333,20 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
@@ -2380,187 +2357,187 @@
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>257</v>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" t="s">
         <v>228</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>229</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>231</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>232</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>233</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C5" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>258</v>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E8" t="s">
-        <v>247</v>
-      </c>
-      <c r="F8">
+        <v>243</v>
+      </c>
+      <c r="F8" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>231</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" t="s">
         <v>248</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>249</v>
       </c>
-      <c r="E10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" t="s">
-        <v>251</v>
-      </c>
-      <c r="D11" t="s">
-        <v>252</v>
-      </c>
-      <c r="E11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D12" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2573,281 +2550,281 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D11" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>277</v>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D12" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D13" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>26</v>
       </c>
       <c r="C14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" t="s">
+        <v>258</v>
+      </c>
+      <c r="D15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" t="s">
         <v>280</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C15" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C18" t="s">
         <v>283</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D18" t="s">
         <v>284</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B19" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" t="s">
         <v>286</v>
       </c>
-      <c r="B17" t="s">
-        <v>282</v>
-      </c>
-      <c r="C17" t="s">
-        <v>262</v>
-      </c>
-      <c r="D17" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D20" t="s">
         <v>287</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" t="s">
+        <v>278</v>
+      </c>
+      <c r="C21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C22" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D22" t="s">
         <v>289</v>
-      </c>
-      <c r="B19" t="s">
-        <v>282</v>
-      </c>
-      <c r="C19" t="s">
-        <v>262</v>
-      </c>
-      <c r="D19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C20" t="s">
-        <v>290</v>
-      </c>
-      <c r="D20" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>184</v>
-      </c>
-      <c r="B21" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" t="s">
-        <v>262</v>
-      </c>
-      <c r="D21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>283</v>
-      </c>
-      <c r="C22" t="s">
-        <v>292</v>
-      </c>
-      <c r="D22" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated readme for JAM
</commit_message>
<xml_diff>
--- a/Brock-et-al_Tables.xlsx
+++ b/Brock-et-al_Tables.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/BCM/Projects/Bike-Injuries/Manuscript/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1054" documentId="8_{BE5EE19E-B02E-485F-AE94-93E3DB24DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3114CCB7-FE1B-4064-9E31-F509F0FC974E}"/>
+  <xr:revisionPtr revIDLastSave="1129" documentId="8_{BE5EE19E-B02E-485F-AE94-93E3DB24DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{588DFDD8-85FE-4A85-9A98-23B94D84489F}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="4" xr2:uid="{45F7941F-18C6-45A1-BF41-0E39AC7E3252}"/>
+    <workbookView xWindow="38280" yWindow="7275" windowWidth="29040" windowHeight="16440" xr2:uid="{45F7941F-18C6-45A1-BF41-0E39AC7E3252}"/>
   </bookViews>
   <sheets>
-    <sheet name="table1_demographics" sheetId="5" r:id="rId1"/>
-    <sheet name="table2_clinical-presentation" sheetId="6" r:id="rId2"/>
-    <sheet name="table3_comorbidities" sheetId="9" r:id="rId3"/>
-    <sheet name="table4_AIS" sheetId="10" r:id="rId4"/>
-    <sheet name="table5_logistic-regression" sheetId="8" r:id="rId5"/>
+    <sheet name="Index" sheetId="11" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="5" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Table 3" sheetId="9" r:id="rId4"/>
+    <sheet name="Table S1" sheetId="10" r:id="rId5"/>
+    <sheet name="Table S2" sheetId="12" r:id="rId6"/>
+    <sheet name="Table S3" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="436">
   <si>
     <t>Male</t>
   </si>
@@ -211,9 +213,6 @@
   </si>
   <si>
     <t>Unplanned Return to OR</t>
-  </si>
-  <si>
-    <t>Substance Abuse Disorder</t>
   </si>
   <si>
     <t>Mental/Personality Disorder</t>
@@ -1214,13 +1213,160 @@
   </si>
   <si>
     <t>1.38 (1.27-1.51, p&lt;0.001)</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Supplemental Digital Content - Table 1</t>
+  </si>
+  <si>
+    <t>Supplemental Digital Content - Table 2</t>
+  </si>
+  <si>
+    <t>Supplemental Digital Content - Table 3</t>
+  </si>
+  <si>
+    <t>Univariable</t>
+  </si>
+  <si>
+    <t>Multivariable</t>
+  </si>
+  <si>
+    <t>OR (95% CI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Helmet (51.3 ± 17.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    No Helmet (43.4 ± 18.9)</t>
+  </si>
+  <si>
+    <t>0.98 (0.98-0.98)</t>
+  </si>
+  <si>
+    <t>(reference)</t>
+  </si>
+  <si>
+    <t>1.30 (1.25-1.37)</t>
+  </si>
+  <si>
+    <t>0.98 (0.94-1.03)</t>
+  </si>
+  <si>
+    <t>5.54 (5.09-6.03)</t>
+  </si>
+  <si>
+    <t>4.25 (3.89-4.66)</t>
+  </si>
+  <si>
+    <t>0.71 (0.65-0.77)</t>
+  </si>
+  <si>
+    <t>0.99 (0.90-1.08)</t>
+  </si>
+  <si>
+    <t>4.18 (3.17-5.61)</t>
+  </si>
+  <si>
+    <t>2.34 (1.73-3.22)</t>
+  </si>
+  <si>
+    <t>1.62 (1.18-2.28)</t>
+  </si>
+  <si>
+    <t>1.50 (1.06-2.16)</t>
+  </si>
+  <si>
+    <t>2.21 (2.07-2.35)</t>
+  </si>
+  <si>
+    <t>1.23 (1.14-1.32)</t>
+  </si>
+  <si>
+    <t>2.95 (2.78-3.12)</t>
+  </si>
+  <si>
+    <t>2.59 (2.42-2.78)</t>
+  </si>
+  <si>
+    <t>3.41 (2.98-3.90)</t>
+  </si>
+  <si>
+    <t>2.50 (2.17-2.89)</t>
+  </si>
+  <si>
+    <t>7.94 (7.34-8.61)</t>
+  </si>
+  <si>
+    <t>5.24 (4.82-5.71)</t>
+  </si>
+  <si>
+    <t>14.36 (12.39-16.76)</t>
+  </si>
+  <si>
+    <t>7.05 (6.04-8.28)</t>
+  </si>
+  <si>
+    <t>7.20 (6.47-8.03)</t>
+  </si>
+  <si>
+    <t>2.08 (1.84-2.36)</t>
+  </si>
+  <si>
+    <t>7.50 (6.98-8.07)</t>
+  </si>
+  <si>
+    <t>4.71 (4.36-5.10)</t>
+  </si>
+  <si>
+    <t>7.30 (6.48-8.26)</t>
+  </si>
+  <si>
+    <t>2.62 (2.29-3.00)</t>
+  </si>
+  <si>
+    <t>1.81 (1.68-1.95)</t>
+  </si>
+  <si>
+    <t>1.38 (1.27-1.51)</t>
+  </si>
+  <si>
+    <t>Demographic Analysis of Pedal-cyclists by Helmet Use</t>
+  </si>
+  <si>
+    <t>Differential Outcomes for Pedal-cyclist Injuries by Intoxication Status</t>
+  </si>
+  <si>
+    <t>Comorbid Conditions for Injured Pedal-Cyclists by Intoxication Status</t>
+  </si>
+  <si>
+    <t>Abbreviated Injury Scale (AIS) Scores in Six Body Regions</t>
+  </si>
+  <si>
+    <t>Logistic Regression for Covariates Linked with Non-Helmet Use</t>
+  </si>
+  <si>
+    <t>Logistic Regression for Covariates Linked with Non-Helmet Use - unformatted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1235,6 +1381,46 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1252,12 +1438,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor rgb="FFD9E1F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1337,11 +1523,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1362,13 +1665,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1377,12 +1673,75 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD9E1F2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1392,10 +1751,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1694,340 +2049,423 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B9346F-9867-4691-989A-5C5E70552A36}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="76.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="B5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="B6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" t="s">
+        <v>435</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Table 1'!A1" display="Table 1" xr:uid="{6E4C0B50-568B-45C7-AC38-0DA6BC0709C2}"/>
+    <hyperlink ref="A3" location="'Table 2'!A1" display="Table 2" xr:uid="{84300E0B-7FCB-48E2-BE36-77A3ADAD575E}"/>
+    <hyperlink ref="A4" location="'Table 3'!A1" display="Table 3" xr:uid="{2E0FD543-68C5-4DB6-8EF2-FB921F2A5E04}"/>
+    <hyperlink ref="A5" location="'Table S1'!A1" display="Supplemental Digital Content - Table 1" xr:uid="{FFE4540E-CC1E-47D4-9EFD-5B5B013C6C41}"/>
+    <hyperlink ref="A6" location="'Table S2'!A1" display="Supplemental Digital Content - Table 2" xr:uid="{43855655-7DE8-4EC7-9F78-BA4E2E8003DA}"/>
+    <hyperlink ref="A7" location="'Table S3'!A1" display="Supplemental Digital Content - Table 3" xr:uid="{71E3D206-E97D-472D-BC1C-3A7CCBDA8C3F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE2C4BC-BC7A-4F93-BCA5-5502F54D71CA}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>77</v>
+      <c r="E1" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>73</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="E2" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="E6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="E8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
       <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="E16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="E22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
       <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="E23" s="5"/>
     </row>
@@ -2037,172 +2475,172 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71AEDE1F-E4AE-413B-AEE4-8AA0C81FA016}">
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>307</v>
+      <c r="G1" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>306</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="G2" s="5">
         <v>0.42699999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
       <c r="B3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>310</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G4" s="5">
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="G6" s="5">
         <v>0.73699999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
       <c r="B7" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -2218,14 +2656,14 @@
         <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2247,131 +2685,131 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>145</v>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>144</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="G10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>80</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="G11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
       <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
       <c r="B14" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
       <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
         <v>167</v>
-      </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
-        <v>168</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>34</v>
@@ -2392,162 +2830,162 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>260</v>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>259</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="G17" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
       <c r="B18" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="G18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
       <c r="B19" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="G19" s="5">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
       <c r="B20" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="G20" s="5">
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
       <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="G21" s="5">
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
       <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>189</v>
-      </c>
       <c r="G22" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
       <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="G23" s="5">
         <v>0.08</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>31</v>
@@ -2556,19 +2994,19 @@
         <v>29</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G24" s="5">
         <v>0.77700000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
       <c r="B25" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>31</v>
@@ -2577,109 +3015,109 @@
         <v>32</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G25" s="5">
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
       <c r="B26" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="G26" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
       <c r="B27" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="G27" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="37"/>
       <c r="B28" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="G28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="37"/>
       <c r="B29" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="G29" s="5">
         <v>0.28399999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F38"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F40"/>
     </row>
   </sheetData>
@@ -2688,497 +3126,336 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7CB57F2-4DBA-4740-A092-F354625704DA}">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="D2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>229</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" s="5">
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15" t="s">
-        <v>60</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="12" t="s">
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>231</v>
       </c>
       <c r="G7" s="5">
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="G9" s="5">
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="37"/>
+      <c r="B11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="5" t="s">
         <v>245</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="G11" s="5">
         <v>0.46500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="F13" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="G14" s="5">
         <v>0.122</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399B2B09-A286-4098-B876-E2221FFBB613}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="G7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3186,64 +3463,726 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399B2B09-A286-4098-B876-E2221FFBB613}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>289</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4DDFDF-AA5D-4944-BFA4-8EC69C4679D6}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34" t="s">
+        <v>396</v>
+      </c>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E10" s="25"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>410</v>
+      </c>
+      <c r="C14" s="25">
+        <v>0</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="E14" s="25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>413</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>415</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E20" s="25"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>419</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>420</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E25" s="25"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>422</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E28" s="25"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E31" s="25"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="E34" s="25"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>429</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E0ABBF-2424-4C90-9AEA-75FDF336C187}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.21875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>325</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>329</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
@@ -3251,37 +4190,37 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>331</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
@@ -3289,109 +4228,109 @@
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>336</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="E9" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="E10" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3399,260 +4338,260 @@
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>353</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>358</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>362</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E16" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="F16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>369</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>371</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>374</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="E20" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="F20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>379</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>380</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="E22" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>384</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>